<commit_message>
Burndown sprint 11, Burndown modulo II
</commit_message>
<xml_diff>
--- a/Documentação/Gráficos Burndown/11ª Sprint/Gráfico Burndown 11.xlsx
+++ b/Documentação/Gráficos Burndown/11ª Sprint/Gráfico Burndown 11.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22413"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cerberus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno Cruz\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEBA3CE2-3BBF-47FE-A38A-6CD76D32F191}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6150" xr2:uid="{880ECEA2-B438-484A-9CBA-91374F2777E2}"/>
+    <workbookView xWindow="1116" yWindow="0" windowWidth="17976" windowHeight="6156"/>
   </bookViews>
   <sheets>
     <sheet name="Atividades" sheetId="1" r:id="rId1"/>
     <sheet name="Burndown" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,8 +86,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,7 +659,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -685,6 +684,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -710,7 +710,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -801,31 +801,31 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FF37-4C89-90CA-991D6049B557}"/>
             </c:ext>
@@ -940,7 +940,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FF37-4C89-90CA-991D6049B557}"/>
             </c:ext>
@@ -956,11 +956,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="605396376"/>
-        <c:axId val="541735776"/>
+        <c:axId val="547445072"/>
+        <c:axId val="547455408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="605396376"/>
+        <c:axId val="547445072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1014,10 +1014,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541735776"/>
+        <c:crossAx val="547455408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1026,7 +1026,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541735776"/>
+        <c:axId val="547455408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1066,10 +1066,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="605396376"/>
+        <c:crossAx val="547445072"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1083,6 +1083,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1108,20 +1109,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1150,7 +1151,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1162,7 +1163,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -1218,7 +1219,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1286,7 +1287,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1297,7 +1298,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1372,7 +1373,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5040-4E13-8C2D-3BC00CF983ED}"/>
             </c:ext>
@@ -1437,7 +1438,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="b"/>
@@ -1448,7 +1449,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1509,7 +1510,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-5040-4E13-8C2D-3BC00CF983ED}"/>
             </c:ext>
@@ -1524,11 +1525,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="605396376"/>
-        <c:axId val="541735776"/>
+        <c:axId val="547457040"/>
+        <c:axId val="547450512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="605396376"/>
+        <c:axId val="547457040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1583,7 +1584,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1620,10 +1621,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541735776"/>
+        <c:crossAx val="547450512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1632,7 +1633,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541735776"/>
+        <c:axId val="547450512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,7 +1702,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1732,10 +1733,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="605396376"/>
+        <c:crossAx val="547457040"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1773,20 +1774,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill flip="none" rotWithShape="1">
@@ -1821,7 +1822,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2949,7 +2950,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5655A40-DE42-43D8-A457-2DC185574AF3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B5655A40-DE42-43D8-A457-2DC185574AF3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2992,7 +2993,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12BD48F8-283C-4952-A38D-C0C427E65D98}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{12BD48F8-283C-4952-A38D-C0C427E65D98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3311,25 +3312,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE633DE-FC74-4926-B2DF-316D2130537E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="9" width="5.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="70.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="9" width="5.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1">
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="31"/>
       <c r="B1" s="31"/>
       <c r="C1" s="25"/>
@@ -3342,7 +3343,7 @@
       <c r="J1" s="26"/>
       <c r="K1" s="27"/>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="34"/>
@@ -3355,7 +3356,7 @@
       <c r="J2" s="26"/>
       <c r="K2" s="27"/>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="29"/>
       <c r="B3" s="29"/>
       <c r="C3" s="34"/>
@@ -3368,7 +3369,7 @@
       <c r="J3" s="26"/>
       <c r="K3" s="27"/>
     </row>
-    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="29"/>
       <c r="B4" s="29"/>
       <c r="C4" s="34"/>
@@ -3381,7 +3382,7 @@
       <c r="J4" s="26"/>
       <c r="K4" s="27"/>
     </row>
-    <row r="5" spans="1:11" ht="97.5" customHeight="1">
+    <row r="5" spans="1:11" ht="97.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="29" t="s">
         <v>0</v>
       </c>
@@ -3396,7 +3397,7 @@
       <c r="J5" s="26"/>
       <c r="K5" s="27"/>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="33" t="s">
         <v>1</v>
       </c>
@@ -3415,7 +3416,7 @@
       </c>
       <c r="K6" s="36"/>
     </row>
-    <row r="7" spans="1:11" ht="45.75" customHeight="1">
+    <row r="7" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3450,7 +3451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" customHeight="1">
+    <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -3460,9 +3461,7 @@
       <c r="C8" s="14">
         <v>1</v>
       </c>
-      <c r="D8" s="15">
-        <v>1</v>
-      </c>
+      <c r="D8" s="15"/>
       <c r="E8" s="14">
         <v>1</v>
       </c>
@@ -3471,15 +3470,15 @@
       <c r="H8" s="15"/>
       <c r="I8" s="14"/>
       <c r="J8" s="19">
-        <f>B8-SUM(C8:I8)</f>
-        <v>-1</v>
+        <f t="shared" ref="J8:J13" si="0">B8-SUM(C8:I8)</f>
+        <v>0</v>
       </c>
       <c r="K8" s="12">
-        <f>IFERROR(1-(J8/B8),"")</f>
-        <v>1.5</v>
+        <f t="shared" ref="K8:K14" si="1">IFERROR(1-(J8/B8),"")</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30" customHeight="1">
+    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -3489,53 +3488,53 @@
       <c r="C9" s="17"/>
       <c r="D9" s="18"/>
       <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
+      <c r="F9" s="18">
+        <v>1</v>
+      </c>
       <c r="G9" s="17">
         <v>1</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="17"/>
       <c r="J9" s="20">
-        <f>B9-SUM(C9:I9)</f>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="12">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K9" s="12">
-        <f>IFERROR(1-(J9/B9),"")</f>
-        <v>0.5</v>
-      </c>
     </row>
-    <row r="10" spans="1:11" ht="30" customHeight="1">
+    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="16">
         <v>2</v>
       </c>
-      <c r="C10" s="17">
-        <v>1</v>
-      </c>
+      <c r="C10" s="17"/>
       <c r="D10" s="18">
         <v>1</v>
       </c>
       <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="17">
+      <c r="F10" s="18">
         <v>1</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="17">
+      <c r="G10" s="17"/>
+      <c r="H10" s="18">
         <v>1</v>
       </c>
+      <c r="I10" s="17"/>
       <c r="J10" s="20">
-        <f>B10-SUM(C10:I10)</f>
-        <v>-2</v>
+        <f t="shared" si="0"/>
+        <v>-1</v>
       </c>
       <c r="K10" s="12">
-        <f>IFERROR(1-(J10/B10),"")</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" customHeight="1">
+    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -3543,53 +3542,51 @@
         <v>1</v>
       </c>
       <c r="C11" s="17"/>
-      <c r="D11" s="18">
-        <v>1</v>
-      </c>
+      <c r="D11" s="18"/>
       <c r="E11" s="17"/>
       <c r="F11" s="18"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="17">
+        <v>2</v>
+      </c>
       <c r="H11" s="18"/>
       <c r="I11" s="17"/>
       <c r="J11" s="20">
-        <f>B11-SUM(C11:I11)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>-1</v>
       </c>
       <c r="K11" s="12">
-        <f>IFERROR(1-(J11/B11),"")</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" customHeight="1">
+    <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="16">
         <v>3</v>
       </c>
-      <c r="C12" s="17">
-        <v>1</v>
-      </c>
-      <c r="D12" s="18">
-        <v>1</v>
-      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="17"/>
       <c r="F12" s="18">
         <v>1</v>
       </c>
       <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
+      <c r="H12" s="18">
+        <v>1</v>
+      </c>
       <c r="I12" s="17"/>
       <c r="J12" s="20">
-        <f>B12-SUM(C12:I12)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="K12" s="12">
-        <f>IFERROR(1-(J12/B12),"")</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30" customHeight="1">
+    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -3597,28 +3594,26 @@
         <v>3</v>
       </c>
       <c r="C13" s="17"/>
-      <c r="D13" s="18">
-        <v>1</v>
-      </c>
+      <c r="D13" s="18"/>
       <c r="E13" s="17"/>
       <c r="F13" s="18"/>
       <c r="G13" s="17">
         <v>1</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="18"/>
+      <c r="I13" s="17">
         <v>1</v>
       </c>
-      <c r="I13" s="17"/>
       <c r="J13" s="20">
-        <f>B13-SUM(C13:I13)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="K13" s="12">
-        <f>IFERROR(1-(J13/B13),"")</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5">
+    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
@@ -3627,43 +3622,43 @@
         <v>13</v>
       </c>
       <c r="C14" s="9">
-        <f>IFERROR(IF(B14-SUM(C8:C13)=B14,NA(),B14-SUM(C8:C13)),NA())</f>
+        <f t="shared" ref="C14:I14" si="2">IFERROR(IF(B14-SUM(C8:C13)=B14,NA(),B14-SUM(C8:C13)),NA())</f>
+        <v>12</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E14" s="9">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="D14" s="9">
-        <f>IFERROR(IF(C14-SUM(D8:D13)=C14,NA(),C14-SUM(D8:D13)),NA())</f>
-        <v>5</v>
-      </c>
-      <c r="E14" s="9">
-        <f>IFERROR(IF(D14-SUM(E8:E13)=D14,NA(),D14-SUM(E8:E13)),NA())</f>
-        <v>4</v>
-      </c>
       <c r="F14" s="9">
-        <f>IFERROR(IF(E14-SUM(F8:F13)=E14,NA(),E14-SUM(F8:F13)),NA())</f>
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="G14" s="9">
-        <f>IFERROR(IF(F14-SUM(G8:G13)=F14,NA(),F14-SUM(G8:G13)),NA())</f>
+      <c r="H14" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="H14" s="9">
-        <f>IFERROR(IF(G14-SUM(H8:H13)=G14,NA(),G14-SUM(H8:H13)),NA())</f>
-        <v>-1</v>
-      </c>
-      <c r="I14" s="9">
-        <f>IFERROR(IF(H14-SUM(I8:I13)=H14,NA(),H14-SUM(I8:I13)),NA())</f>
-        <v>-2</v>
       </c>
       <c r="J14" s="24">
         <f>SUM(J8:J13)</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="K14" s="21">
-        <f>IFERROR(1-(J14/B14),"")</f>
-        <v>1.1538461538461537</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16.5">
+    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
@@ -3672,31 +3667,31 @@
         <v>13</v>
       </c>
       <c r="C15" s="10">
-        <f>IFERROR((IF(B15-($B$14/$G$4) &lt; 0,"-", B15-($B$14/$G$4))),IFERROR(B15-($B$14/7),"-"))</f>
+        <f t="shared" ref="C15:I15" si="3">IFERROR((IF(B15-($B$14/$G$4) &lt; 0,"-", B15-($B$14/$G$4))),IFERROR(B15-($B$14/7),"-"))</f>
         <v>11.142857142857142</v>
       </c>
       <c r="D15" s="10">
-        <f>IFERROR((IF(C15-($B$14/$G$4) &lt; 0,"-", C15-($B$14/$G$4))),IFERROR(C15-($B$14/7),"-"))</f>
+        <f t="shared" si="3"/>
         <v>9.2857142857142847</v>
       </c>
       <c r="E15" s="10">
-        <f>IFERROR((IF(D15-($B$14/$G$4) &lt; 0,"-", D15-($B$14/$G$4))),IFERROR(D15-($B$14/7),"-"))</f>
+        <f t="shared" si="3"/>
         <v>7.428571428571427</v>
       </c>
       <c r="F15" s="10">
-        <f>IFERROR((IF(E15-($B$14/$G$4) &lt; 0,"-", E15-($B$14/$G$4))),IFERROR(E15-($B$14/7),"-"))</f>
+        <f t="shared" si="3"/>
         <v>5.5714285714285694</v>
       </c>
       <c r="G15" s="10">
-        <f>IFERROR((IF(F15-($B$14/$G$4) &lt; 0,"-", F15-($B$14/$G$4))),IFERROR(F15-($B$14/7),"-"))</f>
+        <f t="shared" si="3"/>
         <v>3.7142857142857122</v>
       </c>
       <c r="H15" s="10">
-        <f>IFERROR((IF(G15-($B$14/$G$4) &lt; 0,"-", G15-($B$14/$G$4))),IFERROR(G15-($B$14/7),"-"))</f>
+        <f t="shared" si="3"/>
         <v>1.857142857142855</v>
       </c>
       <c r="I15" s="10">
-        <f>IFERROR((IF(H15-($B$14/$G$4) &lt; 0,"-", H15-($B$14/$G$4))),IFERROR(H15-($B$14/7),"-"))</f>
+        <f t="shared" si="3"/>
         <v>-2.2204460492503131E-15</v>
       </c>
       <c r="J15" s="22"/>
@@ -3757,14 +3752,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACA0E3D-6CA6-4BD2-BA12-8B619DAD9288}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>